<commit_message>
packet length define added.
</commit_message>
<xml_diff>
--- a/임의 정의한 프로토콜.xlsx
+++ b/임의 정의한 프로토콜.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\000. Work\001. FW\Git_ESP32_Server_http_json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924A6163-44C2-422B-AFC5-4176E0D8AB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48EB657-BA4B-4A90-9909-2E04CF8D8BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="1575" windowWidth="20295" windowHeight="13455" xr2:uid="{B3B3D439-A0A4-49F0-9285-1C7CBA6687BE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="15480" xr2:uid="{B3B3D439-A0A4-49F0-9285-1C7CBA6687BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
   <si>
     <t>Start of Text</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -215,102 +215,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2050</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2060</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2070</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2080</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3650</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3660</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3670</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3680</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3690</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3700</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3710</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3720</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5020</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5030</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5040</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5050</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5060</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5070</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5080</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ba5c</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>fe</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Device unique ID_2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>String</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>FF0221FF0B290ACB91A07C9D8D7A36000200010004000200010003205020602070208036503660367036803650366036703680369037003710372050105020503050405050506050705080ba5cfe</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -324,6 +236,82 @@
   </si>
   <si>
     <t>9D8D7A36</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00cd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>816d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0112</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0113</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0114</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0115</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0116</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0117</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0118</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0119</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0069</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0070</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0071</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0072</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dec</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -696,15 +684,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A128D0B2-9F17-4F1B-9C6D-2A87E40B07C7}">
   <dimension ref="C2:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.375" customWidth="1"/>
-    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.625" customWidth="1"/>
     <col min="8" max="8" width="167.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -721,9 +710,12 @@
       <c r="F2" t="s">
         <v>73</v>
       </c>
+      <c r="G2" t="s">
+        <v>74</v>
+      </c>
       <c r="H2" t="str">
         <f>_xlfn.CONCAT(F3:F40)</f>
-        <v>FF0221FF0B290ACB91A07C9D8D7A36000200010004000200010003205020602070208036503660367036803650366036703680369037003710372050105020503050405050506050705080ba5cfe</v>
+        <v>FF0221FF0B290ACB91A07C9D8D7A36000200010004000200010003006900700071007200cd011a16d816d0112011301140115011601170118011901120113011401150116011701180119ba5cFE</v>
       </c>
     </row>
     <row r="3" spans="3:8" x14ac:dyDescent="0.3">
@@ -735,6 +727,10 @@
       </c>
       <c r="F3" s="1" t="s">
         <v>49</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G18" si="0">HEX2DEC(F3)</f>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.3">
@@ -745,8 +741,12 @@
       <c r="F4" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="H4" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.3">
@@ -766,7 +766,11 @@
         <v>4</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>75</v>
+        <v>53</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>4278921482</v>
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.3">
@@ -775,16 +779,24 @@
         <v>5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>76</v>
+        <v>54</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>3415318652</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C8" s="2"/>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>77</v>
+        <v>55</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>2643294774</v>
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.3">
@@ -795,8 +807,8 @@
       <c r="F9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G9" t="str">
-        <f>DEC2HEX(F9)</f>
+      <c r="G9">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -808,6 +820,10 @@
       <c r="F10" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C11" s="2"/>
@@ -817,6 +833,10 @@
       <c r="F11" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C12" s="2"/>
@@ -826,6 +846,10 @@
       <c r="F12" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C13" s="2"/>
@@ -835,6 +859,10 @@
       <c r="F13" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C14" s="2"/>
@@ -844,6 +872,10 @@
       <c r="F14" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C15" s="2"/>
@@ -851,7 +883,11 @@
         <v>12</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>50</v>
+        <v>69</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.3">
@@ -860,208 +896,297 @@
         <v>13</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C17" s="2"/>
       <c r="D17" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C18" s="2"/>
       <c r="D18" t="s">
         <v>15</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>114</v>
+      </c>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C19" s="2"/>
       <c r="D19" t="s">
         <v>16</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="G19">
+        <f>HEX2DEC(F19)</f>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C20" s="2"/>
       <c r="D20" t="s">
         <v>17</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="G20">
+        <f>HEX2DEC(F20)</f>
+        <v>282</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C21" s="2"/>
       <c r="D21" t="s">
         <v>18</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ref="G21:G39" si="1">HEX2DEC(F21)</f>
+        <v>365</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C22" s="2"/>
       <c r="D22" t="s">
         <v>19</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="G22" s="1">
+        <f>32768-(HEX2DEC(F22))</f>
+        <v>-365</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C23" s="2"/>
       <c r="D23" t="s">
         <v>20</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C24" s="2"/>
       <c r="D24" t="s">
         <v>21</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C25" s="2"/>
       <c r="D25" t="s">
         <v>22</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C26" s="2"/>
       <c r="D26" t="s">
         <v>23</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C27" s="2"/>
       <c r="D27" t="s">
         <v>24</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C28" s="2"/>
       <c r="D28" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C29" s="2"/>
       <c r="D29" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C30" s="2"/>
       <c r="D30" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C31" s="2"/>
       <c r="D31" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C32" s="2"/>
       <c r="D32" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C33" s="2"/>
       <c r="D33" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C34" s="2"/>
       <c r="D34" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C35" s="2"/>
       <c r="D35" t="s">
         <v>32</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C36" s="2"/>
       <c r="D36" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C37" s="2"/>
       <c r="D37" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C38" s="2"/>
       <c r="D38" t="s">
         <v>35</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C39" s="2" t="s">
         <v>37</v>
       </c>
@@ -1069,16 +1194,20 @@
         <v>42</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>47708</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C40" s="2"/>
       <c r="D40" t="s">
         <v>38</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>